<commit_message>
Surveys working for the most part
</commit_message>
<xml_diff>
--- a/d09exp/resources/BigFiveQuestions.xlsx
+++ b/d09exp/resources/BigFiveQuestions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sotas\programming\d09exp\d09exp\d09exp\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626E34FC-391F-4EFA-A37D-937838DB77EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FAD2C8-D7E4-4B0B-8098-7BA8B35256AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="58">
   <si>
     <t>Question</t>
   </si>
@@ -163,6 +163,52 @@
   </si>
   <si>
     <t>Id</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>1
+Disagree
+Strongly</t>
+  </si>
+  <si>
+    <t>5
+Agree
+Strongly</t>
+  </si>
+  <si>
+    <t>4
+Agree
+a little</t>
+  </si>
+  <si>
+    <t>2
+Disagree
+a little</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Op1</t>
+  </si>
+  <si>
+    <t>Op2</t>
+  </si>
+  <si>
+    <t>Op3</t>
+  </si>
+  <si>
+    <t>Op4</t>
+  </si>
+  <si>
+    <t>Op5</t>
+  </si>
+  <si>
+    <t>3
+Neither agree
+nor disagree</t>
   </si>
 </sst>
 </file>
@@ -216,13 +262,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,378 +553,1189 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="35.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>45</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C31" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C32" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C34" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C36" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C37" t="s">
+        <v>46</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C38" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C39" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C40" t="s">
+        <v>46</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C41" t="s">
+        <v>46</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C42" t="s">
+        <v>46</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C43" t="s">
+        <v>46</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C44" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C45" t="s">
+        <v>46</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15.4" x14ac:dyDescent="0.45">
       <c r="B47" s="2"/>
     </row>
   </sheetData>

</xml_diff>